<commit_message>
feat: adição de novos vídeos explicativos
</commit_message>
<xml_diff>
--- a/2ª Entrega/03. 2ªEntrega - Cronograma.xlsx
+++ b/2ª Entrega/03. 2ªEntrega - Cronograma.xlsx
@@ -138,22 +138,21 @@
 Preparação para a Apresentação 2.</t>
   </si>
   <si>
-    <t>Implementação avançada: funcionalidades de agenda, frequência, notificações, upload, treino, avaliação física. Refinamento do protótipo
-Início dos testes de unidade e integração.</t>
+    <t>Implementação avançada: funcionalidades de  frequência, notificações, upload de fotos, treino, avaliação física. Refinamento do protótipo. Conexão da tela de criação de instrutor com a API</t>
   </si>
   <si>
     <t>Não iniciada</t>
   </si>
   <si>
-    <t>Continuação da implementação avaçada. Revisão e ajustes de interface e de código conforme feedbacks.
+    <t>Continuação da implementação avaçada, incluindo a criação das telas do usuário do tipo Instrutor. Revisão e ajustes de interface e de código conforme feedbacks, tanto dos stackholders como dos professores.
 Preparação de uma nova versão do documento de requisitos e refinamento dos protótipos de tela.</t>
   </si>
   <si>
     <t>Continuação da implementação avançada. Continuação dos testes do sistema.
-Finalização da modelagem e documentação de requisitos.</t>
-  </si>
-  <si>
-    <t>Conttiuação da implemetnação. Ajustes finais nas funcionalidades e documentação.
+Finalização do documentação de requisitos.</t>
+  </si>
+  <si>
+    <t>Contiuação da implemetnação: ajustes finais nas funcionalidades e documentação.
 Preparação do sistema para avaliação com potenciais usuários.</t>
   </si>
   <si>

</xml_diff>